<commit_message>
Removed typo in BFI-en
</commit_message>
<xml_diff>
--- a/data_raw/dicts/BFI_dict.xlsx
+++ b/data_raw/dicts/BFI_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpipoet\data_raw\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40FCA16-EE9C-4DED-AEB4-2CE8125EA640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D339B2-B9AC-4266-9FC6-DB8E5220F9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BFI_dict" sheetId="1" r:id="rId1"/>
@@ -325,9 +325,6 @@
     <t xml:space="preserve">Ich bin manchmal unhöflich und schroff. </t>
   </si>
   <si>
-    <t>I am sometimes rude to others.)</t>
-  </si>
-  <si>
     <t>Ich neige dazu, Aufgaben vor mir herzuschieben.</t>
   </si>
   <si>
@@ -437,6 +434,9 @@
   </si>
   <si>
     <t>Ich kann mich für Kunst, Musik und Literatur begeistern.</t>
+  </si>
+  <si>
+    <t>I am sometimes rude to others.</t>
   </si>
 </sst>
 </file>
@@ -956,13 +956,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1326,8 +1325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,10 +1350,10 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1366,7 +1365,7 @@
         <v>87</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1377,7 +1376,7 @@
         <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -1389,7 +1388,7 @@
         <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1400,7 +1399,7 @@
         <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1411,7 +1410,7 @@
         <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1422,7 +1421,7 @@
         <v>86</v>
       </c>
       <c r="C8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1444,7 +1443,7 @@
         <v>82</v>
       </c>
       <c r="C10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1455,7 +1454,7 @@
         <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1466,7 +1465,7 @@
         <v>84</v>
       </c>
       <c r="C12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1477,7 +1476,7 @@
         <v>85</v>
       </c>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1488,7 +1487,7 @@
         <v>86</v>
       </c>
       <c r="C14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1510,7 +1509,7 @@
         <v>82</v>
       </c>
       <c r="C16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1521,7 +1520,7 @@
         <v>83</v>
       </c>
       <c r="C17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1532,7 +1531,7 @@
         <v>84</v>
       </c>
       <c r="C18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1543,7 +1542,7 @@
         <v>85</v>
       </c>
       <c r="C19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1554,7 +1553,7 @@
         <v>86</v>
       </c>
       <c r="C20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1576,7 +1575,7 @@
         <v>82</v>
       </c>
       <c r="C22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1587,7 +1586,7 @@
         <v>83</v>
       </c>
       <c r="C23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1598,7 +1597,7 @@
         <v>84</v>
       </c>
       <c r="C24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1609,7 +1608,7 @@
         <v>85</v>
       </c>
       <c r="C25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1620,7 +1619,7 @@
         <v>86</v>
       </c>
       <c r="C26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1642,7 +1641,7 @@
         <v>82</v>
       </c>
       <c r="C28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1653,7 +1652,7 @@
         <v>83</v>
       </c>
       <c r="C29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1664,7 +1663,7 @@
         <v>84</v>
       </c>
       <c r="C30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1675,7 +1674,7 @@
         <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1686,7 +1685,7 @@
         <v>86</v>
       </c>
       <c r="C32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1694,7 +1693,7 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C33" t="s">
         <v>97</v>
@@ -1708,7 +1707,7 @@
         <v>82</v>
       </c>
       <c r="C34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1719,7 +1718,7 @@
         <v>83</v>
       </c>
       <c r="C35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1730,7 +1729,7 @@
         <v>84</v>
       </c>
       <c r="C36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1741,7 +1740,7 @@
         <v>85</v>
       </c>
       <c r="C37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1752,7 +1751,7 @@
         <v>86</v>
       </c>
       <c r="C38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1774,7 +1773,7 @@
         <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1785,7 +1784,7 @@
         <v>83</v>
       </c>
       <c r="C41" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1796,7 +1795,7 @@
         <v>84</v>
       </c>
       <c r="C42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1807,7 +1806,7 @@
         <v>85</v>
       </c>
       <c r="C43" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1818,7 +1817,7 @@
         <v>86</v>
       </c>
       <c r="C44" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1829,7 +1828,7 @@
         <v>100</v>
       </c>
       <c r="C45" t="s">
-        <v>101</v>
+        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1840,7 +1839,7 @@
         <v>82</v>
       </c>
       <c r="C46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1851,7 +1850,7 @@
         <v>83</v>
       </c>
       <c r="C47" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1862,7 +1861,7 @@
         <v>84</v>
       </c>
       <c r="C48" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1873,7 +1872,7 @@
         <v>85</v>
       </c>
       <c r="C49" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1884,7 +1883,7 @@
         <v>86</v>
       </c>
       <c r="C50" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1892,10 +1891,10 @@
         <v>52</v>
       </c>
       <c r="B51" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" t="s">
         <v>102</v>
-      </c>
-      <c r="C51" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1906,7 +1905,7 @@
         <v>82</v>
       </c>
       <c r="C52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1917,7 +1916,7 @@
         <v>83</v>
       </c>
       <c r="C53" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1928,7 +1927,7 @@
         <v>84</v>
       </c>
       <c r="C54" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1939,7 +1938,7 @@
         <v>85</v>
       </c>
       <c r="C55" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1950,7 +1949,7 @@
         <v>86</v>
       </c>
       <c r="C56" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1958,10 +1957,10 @@
         <v>58</v>
       </c>
       <c r="B57" t="s">
+        <v>103</v>
+      </c>
+      <c r="C57" t="s">
         <v>104</v>
-      </c>
-      <c r="C57" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1972,7 +1971,7 @@
         <v>82</v>
       </c>
       <c r="C58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1983,7 +1982,7 @@
         <v>83</v>
       </c>
       <c r="C59" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1994,7 +1993,7 @@
         <v>84</v>
       </c>
       <c r="C60" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -2005,7 +2004,7 @@
         <v>85</v>
       </c>
       <c r="C61" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -2016,7 +2015,7 @@
         <v>86</v>
       </c>
       <c r="C62" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -2024,10 +2023,10 @@
         <v>64</v>
       </c>
       <c r="B63" t="s">
+        <v>105</v>
+      </c>
+      <c r="C63" t="s">
         <v>106</v>
-      </c>
-      <c r="C63" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -2038,18 +2037,18 @@
         <v>82</v>
       </c>
       <c r="C64" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B65" t="s">
         <v>83</v>
       </c>
       <c r="C65" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -2060,7 +2059,7 @@
         <v>84</v>
       </c>
       <c r="C66" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -2071,7 +2070,7 @@
         <v>85</v>
       </c>
       <c r="C67" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -2082,7 +2081,7 @@
         <v>86</v>
       </c>
       <c r="C68" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -2090,10 +2089,10 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
+        <v>107</v>
+      </c>
+      <c r="C69" t="s">
         <v>108</v>
-      </c>
-      <c r="C69" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -2104,7 +2103,7 @@
         <v>82</v>
       </c>
       <c r="C70" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -2115,7 +2114,7 @@
         <v>83</v>
       </c>
       <c r="C71" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -2126,7 +2125,7 @@
         <v>84</v>
       </c>
       <c r="C72" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -2137,7 +2136,7 @@
         <v>85</v>
       </c>
       <c r="C73" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -2148,7 +2147,7 @@
         <v>86</v>
       </c>
       <c r="C74" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -2156,10 +2155,10 @@
         <v>75</v>
       </c>
       <c r="B75" t="s">
+        <v>109</v>
+      </c>
+      <c r="C75" t="s">
         <v>110</v>
-      </c>
-      <c r="C75" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -2170,7 +2169,7 @@
         <v>82</v>
       </c>
       <c r="C76" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -2181,7 +2180,7 @@
         <v>83</v>
       </c>
       <c r="C77" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -2192,7 +2191,7 @@
         <v>84</v>
       </c>
       <c r="C78" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -2203,7 +2202,7 @@
         <v>85</v>
       </c>
       <c r="C79" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -2214,7 +2213,7 @@
         <v>86</v>
       </c>
       <c r="C80" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -2222,142 +2221,142 @@
         <v>81</v>
       </c>
       <c r="B81" t="s">
+        <v>111</v>
+      </c>
+      <c r="C81" t="s">
         <v>112</v>
-      </c>
-      <c r="C81" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B82" t="s">
         <v>82</v>
       </c>
       <c r="C82" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B83" t="s">
         <v>83</v>
       </c>
       <c r="C83" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B84" t="s">
         <v>84</v>
       </c>
       <c r="C84" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B85" t="s">
         <v>85</v>
       </c>
       <c r="C85" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B86" t="s">
         <v>86</v>
       </c>
       <c r="C86" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B87" t="s">
+        <v>119</v>
+      </c>
+      <c r="C87" t="s">
         <v>120</v>
-      </c>
-      <c r="C87" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B88" t="s">
         <v>82</v>
       </c>
       <c r="C88" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B89" t="s">
         <v>83</v>
       </c>
       <c r="C89" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B90" t="s">
         <v>84</v>
       </c>
       <c r="C90" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B91" t="s">
         <v>85</v>
       </c>
       <c r="C91" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B92" t="s">
         <v>86</v>
       </c>
       <c r="C92" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>135</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>123</v>
+        <v>134</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="C93" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed instruction to BFI
</commit_message>
<xml_diff>
--- a/data_raw/dicts/BFI_dict.xlsx
+++ b/data_raw/dicts/BFI_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpipoet\data_raw\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D339B2-B9AC-4266-9FC6-DB8E5220F9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC526D04-4887-40C8-9685-E81801D15C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -376,9 +376,6 @@
     <t>Neither agree, nor disagree</t>
   </si>
   <si>
-    <t>Here are a number of characteristics that may or may not apply to you. For example, do you agree that you are someone who likes to spend time with others? Please write a number next to each statement to indicate the extent to which you agree or disagree with that statement.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ich bin ausgeglichen, nicht leicht aus der Ruhe zu bringen. </t>
   </si>
   <si>
@@ -437,6 +434,9 @@
   </si>
   <si>
     <t>I am sometimes rude to others.</t>
+  </si>
+  <si>
+    <t>Here are a number of characteristics that may or may not apply to you. For example, do you agree that you are someone who likes to spend time with others? Please indicate the extent to which you agree or disagree with that statement.</t>
   </si>
 </sst>
 </file>
@@ -1325,8 +1325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,7 +1351,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C2" t="s">
         <v>88</v>
@@ -1365,7 +1365,7 @@
         <v>87</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1693,7 +1693,7 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C33" t="s">
         <v>97</v>
@@ -1828,7 +1828,7 @@
         <v>100</v>
       </c>
       <c r="C45" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -2042,7 +2042,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B65" t="s">
         <v>83</v>
@@ -2229,7 +2229,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B82" t="s">
         <v>82</v>
@@ -2240,7 +2240,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B83" t="s">
         <v>83</v>
@@ -2251,7 +2251,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B84" t="s">
         <v>84</v>
@@ -2262,7 +2262,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B85" t="s">
         <v>85</v>
@@ -2273,7 +2273,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B86" t="s">
         <v>86</v>
@@ -2284,18 +2284,18 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B87" t="s">
+        <v>118</v>
+      </c>
+      <c r="C87" t="s">
         <v>119</v>
-      </c>
-      <c r="C87" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B88" t="s">
         <v>82</v>
@@ -2306,7 +2306,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B89" t="s">
         <v>83</v>
@@ -2317,7 +2317,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B90" t="s">
         <v>84</v>
@@ -2328,7 +2328,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B91" t="s">
         <v>85</v>
@@ -2339,7 +2339,7 @@
     </row>
     <row r="92" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B92" t="s">
         <v>86</v>
@@ -2350,13 +2350,13 @@
     </row>
     <row r="93" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C93" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>